<commit_message>
Regenerate Excel, and add back to list of files we check
</commit_message>
<xml_diff>
--- a/docs/af/af-metadata.xlsx
+++ b/docs/af/af-metadata.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Export this as TSV" sheetId="1" r:id="rId1"/>
+    <sheet name="Export as TSV" sheetId="1" r:id="rId1"/>
     <sheet name="assay_category list" sheetId="2" r:id="rId2"/>
     <sheet name="assay_type list" sheetId="3" r:id="rId3"/>
     <sheet name="resolution_x_unit list" sheetId="4" r:id="rId4"/>
@@ -775,7 +775,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -855,37 +858,37 @@
     </row>
   </sheetData>
   <dataValidations count="10">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: imaging." sqref="I2:I1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: AF." sqref="J2:J1048576">
       <formula1>'assay_type list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="L2:L1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="O2:O1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="P2:P1048576">
       <formula1>'resolution_x_unit list'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="Q2:Q1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="R2:R1048576">
       <formula1>'resolution_y_unit list'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="S2:S1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="T2:T1048576">
       <formula1>'resolution_z_unit list'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="U2:U1048576">
       <formula1>-2147483647</formula1>
       <formula2>2147483647</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Add version 1 everywhere
</commit_message>
<xml_diff>
--- a/docs/af/af-metadata.xlsx
+++ b/docs/af/af-metadata.xlsx
@@ -8,11 +8,12 @@
   </bookViews>
   <sheets>
     <sheet name="Export as TSV" sheetId="1" r:id="rId1"/>
-    <sheet name="assay_category list" sheetId="2" r:id="rId2"/>
-    <sheet name="assay_type list" sheetId="3" r:id="rId3"/>
-    <sheet name="resolution_x_unit list" sheetId="4" r:id="rId4"/>
-    <sheet name="resolution_y_unit list" sheetId="5" r:id="rId5"/>
-    <sheet name="resolution_z_unit list" sheetId="6" r:id="rId6"/>
+    <sheet name="version list" sheetId="2" r:id="rId2"/>
+    <sheet name="assay_category list" sheetId="3" r:id="rId3"/>
+    <sheet name="assay_type list" sheetId="4" r:id="rId4"/>
+    <sheet name="resolution_x_unit list" sheetId="5" r:id="rId5"/>
+    <sheet name="resolution_y_unit list" sheetId="6" r:id="rId6"/>
+    <sheet name="resolution_z_unit list" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -33,11 +34,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Current version of metadata schema. Template provides the correct value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>HuBMAP Display ID of the donor of the assayed tissue.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -128,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -154,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -167,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -180,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -193,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -206,7 +220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -219,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -232,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -245,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="S1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -258,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="T1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -271,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="U1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -284,7 +298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -297,7 +311,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="W1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -310,7 +324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
+    <comment ref="X1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -323,7 +337,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="Y1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -341,7 +355,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
   <si>
     <t>donor_id</t>
   </si>
@@ -773,7 +793,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -782,33 +802,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>10</v>
@@ -817,78 +837,84 @@
         <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="10">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: imaging." sqref="I2:I1048576">
+  <dataValidations count="11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
+      <formula1>'version list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: imaging." sqref="J2:J1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: AF." sqref="J2:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: AF." sqref="K2:K1048576">
       <formula1>'assay_type list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="L2:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="M2:M1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="O2:O1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="P2:P1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="P2:P1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="Q2:Q1048576">
       <formula1>'resolution_x_unit list'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="Q2:Q1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="R2:R1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="R2:R1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="S2:S1048576">
       <formula1>'resolution_y_unit list'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="S2:S1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="T2:T1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="T2:T1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="U2:U1048576">
       <formula1>'resolution_z_unit list'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="U2:U1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="V2:V1048576">
       <formula1>-2147483647</formula1>
       <formula2>2147483647</formula2>
     </dataValidation>
@@ -908,7 +934,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -936,7 +962,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -944,12 +970,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -967,12 +988,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -990,12 +1011,35 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actually add version numbers to schemas.
</commit_message>
<xml_diff>
--- a/docs/af/af-metadata.xlsx
+++ b/docs/af/af-metadata.xlsx
@@ -8,11 +8,12 @@
   </bookViews>
   <sheets>
     <sheet name="Export as TSV" sheetId="1" r:id="rId1"/>
-    <sheet name="assay_category list" sheetId="2" r:id="rId2"/>
-    <sheet name="assay_type list" sheetId="3" r:id="rId3"/>
-    <sheet name="resolution_x_unit list" sheetId="4" r:id="rId4"/>
-    <sheet name="resolution_y_unit list" sheetId="5" r:id="rId5"/>
-    <sheet name="resolution_z_unit list" sheetId="6" r:id="rId6"/>
+    <sheet name="version list" sheetId="2" r:id="rId2"/>
+    <sheet name="assay_category list" sheetId="3" r:id="rId3"/>
+    <sheet name="assay_type list" sheetId="4" r:id="rId4"/>
+    <sheet name="resolution_x_unit list" sheetId="5" r:id="rId5"/>
+    <sheet name="resolution_y_unit list" sheetId="6" r:id="rId6"/>
+    <sheet name="resolution_z_unit list" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -33,11 +34,37 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Version of the schema to use when validating this metadata.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Free-text description of this assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>HuBMAP Display ID of the donor of the assayed tissue.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -128,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -154,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -167,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -180,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -193,7 +220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -206,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -219,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -232,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="S1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -245,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="T1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -258,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="U1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -271,7 +298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -284,7 +311,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="W1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -297,7 +324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="X1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -310,7 +337,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
+    <comment ref="Y1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -323,7 +350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="Z1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -341,7 +368,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
   <si>
     <t>donor_id</t>
   </si>
@@ -773,7 +809,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -782,113 +818,122 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="10">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: imaging." sqref="I2:I1048576">
+  <dataValidations count="11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
+      <formula1>'version list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: imaging." sqref="K2:K1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: AF." sqref="J2:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: AF." sqref="L2:L1048576">
       <formula1>'assay_type list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="L2:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="N2:N1048576">
       <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="O2:O1048576">
-      <formula1>-1e+307</formula1>
-      <formula2>1e+307</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="P2:P1048576">
-      <formula1>'resolution_x_unit list'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="Q2:Q1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="R2:R1048576">
-      <formula1>'resolution_y_unit list'!$A$1:$A$2</formula1>
+      <formula1>'resolution_x_unit list'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="S2:S1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="T2:T1048576">
+      <formula1>'resolution_y_unit list'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="U2:U1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="V2:V1048576">
       <formula1>'resolution_z_unit list'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="U2:U1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="W2:W1048576">
       <formula1>-2147483647</formula1>
       <formula2>2147483647</formula2>
     </dataValidation>
@@ -908,7 +953,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -926,7 +971,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -936,7 +981,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -944,12 +989,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -967,12 +1007,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -990,12 +1030,35 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
assays version 1 (#635)
* assays version 1

* regen

* Should be git-ignored

* Add built yamls

* Actually add version numbers to schemas.

* Add is_contact; Fix #604

* Remove start/end datetimes from IMC. Fix #561.

* antibodies_path in IMC. Fix #551

* update descriptions list

* For the good fixtures, add a v1
</commit_message>
<xml_diff>
--- a/docs/af/af-metadata.xlsx
+++ b/docs/af/af-metadata.xlsx
@@ -8,11 +8,12 @@
   </bookViews>
   <sheets>
     <sheet name="Export as TSV" sheetId="1" r:id="rId1"/>
-    <sheet name="assay_category list" sheetId="2" r:id="rId2"/>
-    <sheet name="assay_type list" sheetId="3" r:id="rId3"/>
-    <sheet name="resolution_x_unit list" sheetId="4" r:id="rId4"/>
-    <sheet name="resolution_y_unit list" sheetId="5" r:id="rId5"/>
-    <sheet name="resolution_z_unit list" sheetId="6" r:id="rId6"/>
+    <sheet name="version list" sheetId="2" r:id="rId2"/>
+    <sheet name="assay_category list" sheetId="3" r:id="rId3"/>
+    <sheet name="assay_type list" sheetId="4" r:id="rId4"/>
+    <sheet name="resolution_x_unit list" sheetId="5" r:id="rId5"/>
+    <sheet name="resolution_y_unit list" sheetId="6" r:id="rId6"/>
+    <sheet name="resolution_z_unit list" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -33,11 +34,37 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Version of the schema to use when validating this metadata.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Free-text description of this assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>HuBMAP Display ID of the donor of the assayed tissue.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -128,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -154,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -167,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -180,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -193,7 +220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -206,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -219,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -232,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="S1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -245,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="T1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -258,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="U1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -271,7 +298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -284,7 +311,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="W1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -297,7 +324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="X1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -310,7 +337,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
+    <comment ref="Y1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -323,7 +350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="Z1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -341,7 +368,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
   <si>
     <t>donor_id</t>
   </si>
@@ -773,7 +809,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -782,113 +818,122 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="10">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: imaging." sqref="I2:I1048576">
+  <dataValidations count="11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
+      <formula1>'version list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: imaging." sqref="K2:K1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: AF." sqref="J2:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: AF." sqref="L2:L1048576">
       <formula1>'assay_type list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="L2:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="N2:N1048576">
       <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="O2:O1048576">
-      <formula1>-1e+307</formula1>
-      <formula2>1e+307</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="P2:P1048576">
-      <formula1>'resolution_x_unit list'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="Q2:Q1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="R2:R1048576">
-      <formula1>'resolution_y_unit list'!$A$1:$A$2</formula1>
+      <formula1>'resolution_x_unit list'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="S2:S1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="T2:T1048576">
+      <formula1>'resolution_y_unit list'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="U2:U1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="V2:V1048576">
       <formula1>'resolution_z_unit list'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="U2:U1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="W2:W1048576">
       <formula1>-2147483647</formula1>
       <formula2>2147483647</formula2>
     </dataValidation>
@@ -908,7 +953,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -926,7 +971,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -936,7 +981,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -944,12 +989,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -967,12 +1007,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -990,12 +1030,35 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
factor out resolution_z_unit (#817)
* factor out resolution_z_unit

* Update src/ingest_validation_tools/table-schemas/includes/fields/resolution_z_unit.yaml

Co-authored-by: chris briggs <cebriggs7135@gmail.com>

* Apply suggestions from code review

* Regen

Co-authored-by: chris briggs <cebriggs7135@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/af/af-metadata.xlsx
+++ b/docs/af/af-metadata.xlsx
@@ -307,7 +307,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The unit of incremental distance between image slices.(um)</t>
+          <t>The unit of incremental distance between image slices.</t>
         </r>
       </text>
     </comment>
@@ -368,7 +368,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>version</t>
   </si>
@@ -449,6 +449,9 @@
   </si>
   <si>
     <t>resolution_z_unit</t>
+  </si>
+  <si>
+    <t>mm</t>
   </si>
   <si>
     <t>number_of_channels</t>
@@ -886,16 +889,16 @@
         <v>26</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -930,8 +933,8 @@
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="V2:V1048576">
-      <formula1>'resolution_z_unit list'!$A$1:$A$2</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: mm / um / nm." sqref="V2:V1048576">
+      <formula1>'resolution_z_unit list'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="W2:W1048576">
       <formula1>-2147483647</formula1>
@@ -1045,7 +1048,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1053,12 +1056,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
regen / fix tests
</commit_message>
<xml_diff>
--- a/docs/af/af-metadata.xlsx
+++ b/docs/af/af-metadata.xlsx
@@ -11,9 +11,10 @@
     <sheet name="version list" sheetId="2" r:id="rId2"/>
     <sheet name="assay_category list" sheetId="3" r:id="rId3"/>
     <sheet name="assay_type list" sheetId="4" r:id="rId4"/>
-    <sheet name="resolution_x_unit list" sheetId="5" r:id="rId5"/>
-    <sheet name="resolution_y_unit list" sheetId="6" r:id="rId6"/>
-    <sheet name="resolution_z_unit list" sheetId="7" r:id="rId7"/>
+    <sheet name="is_targeted list" sheetId="5" r:id="rId5"/>
+    <sheet name="resolution_x_unit list" sheetId="6" r:id="rId6"/>
+    <sheet name="resolution_y_unit list" sheetId="7" r:id="rId7"/>
+    <sheet name="resolution_z_unit list" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -368,7 +369,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>version</t>
   </si>
@@ -419,6 +420,12 @@
   </si>
   <si>
     <t>is_targeted</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
   <si>
     <t>acquisition_instrument_vendor</t>
@@ -865,40 +872,40 @@
         <v>16</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -912,8 +919,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: AF." sqref="L2:L1048576">
       <formula1>'assay_type list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="N2:N1048576">
-      <formula1>"TRUE,FALSE"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: TRUE / FALSE." sqref="N2:N1048576">
+      <formula1>'is_targeted list'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="Q2:Q1048576">
       <formula1>-1e+307</formula1>
@@ -1010,12 +1017,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1033,12 +1040,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1047,6 +1054,29 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -1056,17 +1086,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>